<commit_message>
Update journal de travail James
</commit_message>
<xml_diff>
--- a/Dossiers personnels/James/Journal_Travail.xlsx
+++ b/Dossiers personnels/James/Journal_Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t xml:space="preserve">Journal de travail</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Suivit du tutoriel sur Java FX de openClassroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation de la main frame</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -70,7 +73,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY;@"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -312,7 +315,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -435,10 +438,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="n">
+        <v>43178</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
@@ -532,11 +541,11 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="10" t="n">
         <f aca="false">SUM(C5:C31)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail James et WindowsNewProject fmxl created
</commit_message>
<xml_diff>
--- a/Dossiers personnels/James/Journal_Travail.xlsx
+++ b/Dossiers personnels/James/Journal_Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t xml:space="preserve">Journal de travail</t>
   </si>
@@ -62,6 +62,18 @@
   </si>
   <si>
     <t xml:space="preserve">Réalisation de la main frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussion, planification et organisation de groupe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conception et analyse de la drawZone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brainstrom et résolution de bug graphique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du projet sur IceScrum (prend trop de temps : abondon)</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -315,7 +327,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -449,25 +461,49 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
+        <v>43185</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="n">
+        <v>43185</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
+        <v>43199</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <v>43205</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6"/>
@@ -541,11 +577,11 @@
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C32" s="10" t="n">
         <f aca="false">SUM(C5:C31)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail :3
</commit_message>
<xml_diff>
--- a/Dossiers personnels/James/Journal_Travail.xlsx
+++ b/Dossiers personnels/James/Journal_Travail.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t xml:space="preserve">Journal de travail</t>
   </si>
@@ -61,7 +61,124 @@
     <t xml:space="preserve">Suivit du tutoriel sur Java FX de openClassroom</t>
   </si>
   <si>
-    <t xml:space="preserve">Réalisation de la main frame</t>
+    <t xml:space="preserve">Réalisation de la main frame (fenêtre principale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation du menu de droite (calque + historique UI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussion, planification et organisation de groupe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture de la documentation sur les Canvas JavaFX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test des canvas JavaFX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de la drawZone (zone ou on va dessiner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du fxml pour la pop up pour les nouveaux projets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du controleur pour le fenêtre pour les nouveau projets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug pencil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création du fxml et du controler pour la bar des paramètres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout de la paramBar au fxml principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création des fxml pour les outils pinceau, gomme, rognage, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug des params bars (illegal argument)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactor et renommage des params bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des racourcis clavier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des éléments dans la liste des calques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug addNewLayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développement de l’outil bucketFill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développement de l’outil TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug TextTool et bucketFill (undo redo principalement)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug TextTool et bucketFill (suite)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug paramBar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développement de l’outil Crop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug Crop et TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug Crop + undo redo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commentaire et debug Crop/TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changement dans les calques temporaire Crop/TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug pencil et eraser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des ToolTips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des couleurs pour le TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug bucketFill (plus rapide)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug shape (on clic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add undo/redo TextTOol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add undo/redo import Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add undo/redo new/open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add commentaire (nouveau format) sur main/UndoException/utils/windowsNewProject/MenuBar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug TextTool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug scollBar history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout des curseurs pour tous les outils</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rapport</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -75,7 +192,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -120,6 +237,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -190,7 +313,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,11 +350,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,10 +439,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,106 +573,484 @@
         <v>13</v>
       </c>
       <c r="C13" s="8" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="n">
+        <v>43178</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="10" t="n">
-        <f aca="false">SUM(C5:C31)</f>
+      <c r="C14" s="8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="n">
+        <v>43185</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="n">
+        <v>43187</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="n">
+        <v>43187</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="n">
+        <v>43199</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="n">
+        <v>43205</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="n">
+        <v>43205</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="n">
+        <v>43205</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>21</v>
+      </c>
+      <c r="C21" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="n">
+        <v>43218</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="n">
+        <v>43218</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="8" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
+        <v>43218</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
+        <v>43220</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
+        <v>43220</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
+        <v>43220</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
+        <v>43220</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
+        <v>43220</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
+        <v>43221</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="n">
+        <v>43230</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="8" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="n">
+        <v>43230</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="8" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="n">
+        <v>43230</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="8" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="n">
+        <v>43231</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="n">
+        <v>43231</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="n">
+        <v>43231</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="n">
+        <v>43234</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="n">
+        <v>43234</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="n">
+        <v>43236</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="n">
+        <v>43236</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="n">
+        <v>43236</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="n">
+        <v>43236</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="6" t="n">
+        <v>43236</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="8" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="6" t="n">
+        <v>43237</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="6" t="n">
+        <v>43238</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="8" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="6" t="n">
+        <v>43238</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="6" t="n">
+        <v>43238</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="6" t="n">
+        <v>43240</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="6"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="6"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="11" t="n">
+        <f aca="false">SUM(C5:C58)</f>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>